<commit_message>
#Progress of changing the calculate function and data_processing_from_coordinate
</commit_message>
<xml_diff>
--- a/Data Kapal Kriso KCS.xlsx
+++ b/Data Kapal Kriso KCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Phyton\TES MESIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\PycharmProjects\TES MESIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC7E182-0AD6-4316-A7C8-26EEBBDA6E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F489ADA0-700C-43D6-8D0F-FC138A62FE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A4AF8467-32B8-45D2-AA35-F36288F8BE18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A4AF8467-32B8-45D2-AA35-F36288F8BE18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -715,18 +715,18 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -736,7 +736,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -748,7 +748,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -760,7 +760,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -784,7 +784,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -798,7 +798,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -812,7 +812,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -826,7 +826,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -854,7 +854,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -868,7 +868,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -880,7 +880,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -892,7 +892,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -901,18 +901,18 @@
       </c>
       <c r="C14" s="11"/>
     </row>
-    <row r="15" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="21">
-        <v>14400</v>
+        <v>25000</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -923,7 +923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -951,12 +951,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -970,7 +970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -984,7 +984,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -998,7 +998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>

</xml_diff>